<commit_message>
add new huong dan
</commit_message>
<xml_diff>
--- a/Huong dẫn dùng trang WEB_qmloffice.site.xlsx
+++ b/Huong dẫn dùng trang WEB_qmloffice.site.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\WEB\QMLAdmin\3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\WEB\QMLAdmin\html_office\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0414C3A-D8BD-40C5-A0D6-C69507F76B0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5339B811-BC06-451B-BDAB-BAF11DBB0B83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="trang quản lí nhân sự" sheetId="1" r:id="rId1"/>
     <sheet name="TRANG QUẢN LÍ CHÍNH" sheetId="2" r:id="rId2"/>
     <sheet name="Chi tiết công việc" sheetId="3" r:id="rId3"/>
+    <sheet name="Phần list công việc of USER" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -457,15 +458,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>607362</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>122819</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -481,7 +482,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2819400" y="2838450"/>
+          <a:off x="2209800" y="1314450"/>
           <a:ext cx="17904762" cy="8190494"/>
           <a:chOff x="3048000" y="2952750"/>
           <a:chExt cx="17904762" cy="8047619"/>
@@ -550,15 +551,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>607370</xdr:colOff>
-      <xdr:row>102</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>189462</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -594,15 +595,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>90</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -647,15 +648,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>152399</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -730,15 +731,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -798,15 +799,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>112</xdr:row>
+      <xdr:row>104</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>455467</xdr:colOff>
-      <xdr:row>149</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>18167</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -847,15 +848,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>398318</xdr:colOff>
-      <xdr:row>116</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>17317</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>155864</xdr:colOff>
-      <xdr:row>277</xdr:row>
+      <xdr:row>164</xdr:row>
       <xdr:rowOff>34636</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -897,15 +898,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>432706</xdr:colOff>
-      <xdr:row>277</xdr:row>
+      <xdr:row>164</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>42181</xdr:colOff>
-      <xdr:row>316</xdr:row>
+      <xdr:row>203</xdr:row>
       <xdr:rowOff>40821</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -947,10 +948,10 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>328814</xdr:colOff>
-      <xdr:row>316</xdr:row>
-      <xdr:rowOff>64585</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>166889</xdr:colOff>
+      <xdr:row>206</xdr:row>
+      <xdr:rowOff>16960</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="12044161" cy="1888040"/>
     <xdr:sp macro="" textlink="">
@@ -966,7 +967,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16178414" y="60262585"/>
+          <a:off x="776489" y="39259960"/>
           <a:ext cx="12044161" cy="1888040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1103,6 +1104,61 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D11B58D0-CE78-40AC-A138-038FC289E36C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609599" y="380999"/>
+          <a:ext cx="14544675" cy="10791825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1371,7 +1427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:AJ61"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1450,84 +1506,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{461F61A3-F414-43C8-8A65-8907EB4168DA}">
-  <dimension ref="C9:T110"/>
+  <dimension ref="B1:S102"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B122" sqref="B122"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="9" spans="4:19" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="D9" s="3" t="s">
+    <row r="1" spans="3:18" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
     </row>
-    <row r="12" spans="4:19" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="E12" s="3" t="s">
+    <row r="4" spans="3:18" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
     </row>
-    <row r="54" spans="6:14" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
+    <row r="46" spans="5:13" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
     </row>
-    <row r="110" spans="3:20" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C110" s="3" t="s">
+    <row r="102" spans="2:19" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B102" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D110" s="4"/>
-      <c r="E110" s="4"/>
-      <c r="F110" s="4"/>
-      <c r="G110" s="2"/>
-      <c r="H110" s="2"/>
-      <c r="I110" s="2"/>
-      <c r="J110" s="2"/>
-      <c r="K110" s="2"/>
-      <c r="L110" s="2"/>
-      <c r="M110" s="2"/>
-      <c r="N110" s="2"/>
-      <c r="O110" s="2"/>
-      <c r="P110" s="2"/>
-      <c r="Q110" s="1"/>
-      <c r="R110" s="1"/>
-      <c r="S110" s="1"/>
-      <c r="T110" s="1"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
+      <c r="L102" s="2"/>
+      <c r="M102" s="2"/>
+      <c r="N102" s="2"/>
+      <c r="O102" s="2"/>
+      <c r="P102" s="1"/>
+      <c r="Q102" s="1"/>
+      <c r="R102" s="1"/>
+      <c r="S102" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1539,9 +1593,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A24C2D9-6755-4EF1-84A5-CDAF62410FB3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A275" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q327" sqref="Q327"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E6CA26-7BB9-4714-809B-2404741838AA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>